<commit_message>
Changes. It's been too long to remember.
</commit_message>
<xml_diff>
--- a/weather sensor power consuption.xlsx
+++ b/weather sensor power consuption.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jbellows\Documents\Arduino\WindStation\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="18195" windowHeight="7995"/>
   </bookViews>
@@ -11,7 +16,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -21,7 +26,7 @@
     <author>James Brown</author>
   </authors>
   <commentList>
-    <comment ref="L4" authorId="0">
+    <comment ref="M4" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -29,7 +34,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>James Brown:</t>
         </r>
@@ -38,14 +43,14 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Days if we only get 65% of the listed battery capacity</t>
         </r>
       </text>
     </comment>
-    <comment ref="M4" authorId="0">
+    <comment ref="N4" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -53,7 +58,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>James Brown:</t>
         </r>
@@ -62,14 +67,14 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Days if we only get 50% of the listed battery capacity</t>
         </r>
       </text>
     </comment>
-    <comment ref="D8" authorId="0">
+    <comment ref="D8" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -77,7 +82,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>James Brown:</t>
         </r>
@@ -86,7 +91,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 200 ms every 5 minutes</t>
@@ -98,7 +103,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Weather station power consumption calculations</t>
   </si>
@@ -170,6 +175,9 @@
   </si>
   <si>
     <t>AAA</t>
+  </si>
+  <si>
+    <t>Days @ 80%</t>
   </si>
 </sst>
 </file>
@@ -188,14 +196,14 @@
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -230,6 +238,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -278,7 +289,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -313,7 +324,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -522,31 +533,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M13"/>
+  <dimension ref="A1:N13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M4" sqref="M4"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="9" max="9" width="15.5703125" customWidth="1"/>
     <col min="10" max="11" width="7.85546875" customWidth="1"/>
-    <col min="12" max="12" width="12.28515625" customWidth="1"/>
-    <col min="13" max="13" width="11.5703125" customWidth="1"/>
+    <col min="12" max="12" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.28515625" customWidth="1"/>
+    <col min="14" max="14" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -575,18 +587,21 @@
         <v>9</v>
       </c>
       <c r="L4" t="s">
+        <v>24</v>
+      </c>
+      <c r="M4" t="s">
         <v>21</v>
       </c>
-      <c r="M4" t="s">
+      <c r="N4" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>16</v>
       </c>
       <c r="B5">
-        <v>6</v>
+        <v>120</v>
       </c>
       <c r="C5">
         <v>100000</v>
@@ -596,7 +611,7 @@
       </c>
       <c r="E5">
         <f>((D5*C5) + ((1000-D5)*B5))/1000</f>
-        <v>55.997</v>
+        <v>169.94</v>
       </c>
       <c r="H5" t="s">
         <v>10</v>
@@ -606,22 +621,26 @@
       </c>
       <c r="J5" s="1">
         <f>I5/($E$13/1000)</f>
-        <v>4724.3018934524307</v>
+        <v>4426.4966944398184</v>
       </c>
       <c r="K5" s="1">
         <f>J5/24</f>
-        <v>196.84591222718461</v>
+        <v>184.43736226832576</v>
       </c>
       <c r="L5" s="1">
+        <f>K5*0.8</f>
+        <v>147.54988981466062</v>
+      </c>
+      <c r="M5" s="1">
         <f>K5*0.65</f>
-        <v>127.94984294767001</v>
-      </c>
-      <c r="M5" s="1">
+        <v>119.88428547441174</v>
+      </c>
+      <c r="N5" s="1">
         <f>K5*0.5</f>
-        <v>98.422956113592306</v>
+        <v>92.218681134162878</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -632,12 +651,12 @@
         <v>100</v>
       </c>
       <c r="D6">
-        <f>200/(5*60*1000)</f>
-        <v>6.6666666666666664E-4</v>
+        <f>200/(1*60*1000)</f>
+        <v>3.3333333333333335E-3</v>
       </c>
       <c r="E6">
         <f t="shared" ref="E6:E8" si="0">((D6*C6) + ((1000-D6)*B6))/1000</f>
-        <v>2.0000653333333331</v>
+        <v>2.0003266666666666</v>
       </c>
       <c r="H6" t="s">
         <v>11</v>
@@ -647,34 +666,41 @@
       </c>
       <c r="J6" s="1">
         <f t="shared" ref="J6:J9" si="1">I6/($E$13/1000)</f>
-        <v>15747.672978174769</v>
+        <v>14754.988981466062</v>
       </c>
       <c r="K6" s="1">
         <f t="shared" ref="K6:K9" si="2">J6/24</f>
-        <v>656.15304075728204</v>
+        <v>614.79120756108591</v>
       </c>
       <c r="L6" s="1">
-        <f t="shared" ref="L6:L9" si="3">K6*0.65</f>
-        <v>426.49947649223333</v>
+        <f>K6*0.8</f>
+        <v>491.83296604886874</v>
       </c>
       <c r="M6" s="1">
-        <f t="shared" ref="M6:M9" si="4">K6*0.5</f>
-        <v>328.07652037864102</v>
+        <f t="shared" ref="M6:M9" si="3">K6*0.65</f>
+        <v>399.61428491470588</v>
+      </c>
+      <c r="N6" s="1">
+        <f t="shared" ref="N6:N9" si="4">K6*0.5</f>
+        <v>307.39560378054296</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>14</v>
       </c>
       <c r="B7">
-        <v>200</v>
+        <v>120</v>
       </c>
       <c r="C7">
-        <v>1500</v>
+        <v>120</v>
+      </c>
+      <c r="D7">
+        <v>500</v>
       </c>
       <c r="E7">
         <f t="shared" si="0"/>
-        <v>200</v>
+        <v>120</v>
       </c>
       <c r="H7" t="s">
         <v>12</v>
@@ -684,22 +710,26 @@
       </c>
       <c r="J7" s="1">
         <f t="shared" si="1"/>
-        <v>33463.805078621386</v>
+        <v>31354.351585615383</v>
       </c>
       <c r="K7" s="1">
         <f t="shared" si="2"/>
-        <v>1394.3252116092244</v>
+        <v>1306.4313160673075</v>
       </c>
       <c r="L7" s="1">
+        <f>K7*0.8</f>
+        <v>1045.145052853846</v>
+      </c>
+      <c r="M7" s="1">
         <f t="shared" si="3"/>
-        <v>906.3113875459959</v>
-      </c>
-      <c r="M7" s="1">
+        <v>849.18035544374993</v>
+      </c>
+      <c r="N7" s="1">
         <f t="shared" si="4"/>
-        <v>697.16260580461221</v>
+        <v>653.21565803365377</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -707,15 +737,15 @@
         <v>250</v>
       </c>
       <c r="C8">
-        <v>22000</v>
+        <v>75000</v>
       </c>
       <c r="D8">
-        <f>200/(5*60*1000)</f>
-        <v>6.6666666666666664E-4</v>
+        <f>200/(1*60*1000)</f>
+        <v>3.3333333333333335E-3</v>
       </c>
       <c r="E8">
         <f t="shared" si="0"/>
-        <v>250.01449999999997</v>
+        <v>250.24916666666667</v>
       </c>
       <c r="H8" t="s">
         <v>19</v>
@@ -725,22 +755,26 @@
       </c>
       <c r="J8" s="1">
         <f t="shared" si="1"/>
-        <v>885.80660502233081</v>
+        <v>829.96813020746595</v>
       </c>
       <c r="K8" s="1">
         <f t="shared" si="2"/>
-        <v>36.908608542597115</v>
+        <v>34.582005425311081</v>
       </c>
       <c r="L8" s="1">
+        <f>K8*0.8</f>
+        <v>27.665604340248866</v>
+      </c>
+      <c r="M8" s="1">
         <f t="shared" si="3"/>
-        <v>23.990595552688127</v>
-      </c>
-      <c r="M8" s="1">
+        <v>22.478303526452205</v>
+      </c>
+      <c r="N8" s="1">
         <f t="shared" si="4"/>
-        <v>18.454304271298557</v>
+        <v>17.291002712655541</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="H9" t="s">
         <v>23</v>
       </c>
@@ -749,28 +783,32 @@
       </c>
       <c r="J9" s="1">
         <f t="shared" si="1"/>
-        <v>2263.7279906126232</v>
+        <v>2121.0296660857462</v>
       </c>
       <c r="K9" s="1">
         <f t="shared" si="2"/>
-        <v>94.321999608859301</v>
+        <v>88.37623608690609</v>
       </c>
       <c r="L9" s="1">
+        <f>K9*0.8</f>
+        <v>70.700988869524878</v>
+      </c>
+      <c r="M9" s="1">
         <f t="shared" si="3"/>
-        <v>61.309299745758544</v>
-      </c>
-      <c r="M9" s="1">
+        <v>57.444553456488961</v>
+      </c>
+      <c r="N9" s="1">
         <f t="shared" si="4"/>
-        <v>47.16099980442965</v>
+        <v>44.188118043453045</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>17</v>
       </c>
       <c r="E13">
         <f>SUM(E5:E12)</f>
-        <v>508.01156533333335</v>
+        <v>542.1894933333333</v>
       </c>
       <c r="F13" t="s">
         <v>18</v>

</xml_diff>